<commit_message>
Re-publish to correct Location
</commit_message>
<xml_diff>
--- a/docs/UKCore-Location.xlsx
+++ b/docs/UKCore-Location.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="366">
   <si>
     <t>Path</t>
   </si>
@@ -1148,10 +1148,6 @@
   </si>
   <si>
     <t>Location.endpoint.identifier.assigner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Organization|https://fhir.nhs.uk/R4/StructureDefinition/UKCore-Organization)
-</t>
   </si>
   <si>
     <t>Location.endpoint.display</t>
@@ -10713,7 +10709,7 @@
         <v>47</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>365</v>
+        <v>168</v>
       </c>
       <c r="K90" t="s" s="2">
         <v>169</v>
@@ -10795,7 +10791,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">

</xml_diff>